<commit_message>
corrections to orig dataset & chaos
</commit_message>
<xml_diff>
--- a/src/raw_data/TG_errors.xlsx
+++ b/src/raw_data/TG_errors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tjasagrabnar/Desktop/magistrska/customer_data_cleanup/src/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBAA1C54-DC22-4F4F-92F3-EFD22F7F1A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F54713-F3DD-2042-888F-24CBB9BE2436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17180" yWindow="1020" windowWidth="16880" windowHeight="21080" xr2:uid="{AE53E973-26AC-D344-B98A-BA50389E6E12}"/>
+    <workbookView xWindow="17160" yWindow="1020" windowWidth="16880" windowHeight="21080" xr2:uid="{AE53E973-26AC-D344-B98A-BA50389E6E12}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$1:$I$81</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$1:$I$84</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="253">
   <si>
     <t>Error_ID</t>
   </si>
@@ -239,9 +239,6 @@
   </si>
   <si>
     <t>here also important to note that the house number cannot just be deleted, because it may be missing in the house_number column</t>
-  </si>
-  <si>
-    <t>not actually duplicates + here also important to note that the house number cannot just be deleted, because it may be missing in the house_number column</t>
   </si>
   <si>
     <t>Ljubljana 1000</t>
@@ -823,12 +820,15 @@
   <si>
     <t>More than 4</t>
   </si>
+  <si>
+    <t>DOE</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -879,8 +879,21 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -890,6 +903,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -917,12 +935,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
@@ -965,9 +984,14 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="3" builtinId="27"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="1" builtinId="10"/>
@@ -1302,11 +1326,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E25534D8-8326-A74F-A2E5-C7F409A5D2ED}">
-  <dimension ref="A1:J84"/>
+  <dimension ref="A1:J87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1324,13 +1348,13 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -1342,30 +1366,30 @@
         <v>37</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>114</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J1" s="15" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
-        <v>4101</v>
+        <v>1101</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>31</v>
+        <v>93</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>144</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>31</v>
@@ -1377,63 +1401,65 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
-        <v>4101</v>
+        <v>1102</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>4</v>
+        <v>69</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>30</v>
+        <v>93</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="3"/>
+        <v>94</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="J3">
         <v>0.05</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
-        <v>4102</v>
+        <v>1103</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>70</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>33</v>
+        <v>93</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>95</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="J4">
         <v>0.02</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
-        <v>4201</v>
+        <v>1104</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>4</v>
+        <v>71</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>31</v>
+        <v>93</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>96</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>31</v>
+        <v>94</v>
       </c>
       <c r="F5" s="3"/>
       <c r="J5">
@@ -1442,41 +1468,41 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
-        <v>4201</v>
+        <v>1105</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>30</v>
+        <v>93</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>117</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="3"/>
+        <v>94</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="J6">
         <v>0.05</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
-        <v>4202</v>
+        <v>1106</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" s="3">
-        <v>2</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="J7">
         <v>0.02</v>
@@ -1484,45 +1510,43 @@
     </row>
     <row r="8" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
-        <v>4301</v>
+        <v>1201</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>152</v>
+        <v>97</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>151</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>83</v>
-      </c>
+      <c r="F8" s="3"/>
       <c r="J8">
         <v>0.01</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
-        <v>4203</v>
+        <v>1202</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>235</v>
+        <v>69</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>48</v>
+        <v>97</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>109</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>31</v>
+        <v>98</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="J9">
         <v>0.01</v>
@@ -1530,154 +1554,144 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
-        <v>3105</v>
+        <v>1203</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>165</v>
+        <v>70</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="E10" s="3"/>
+        <v>97</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="F10" s="3" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="J10">
         <v>0.05</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
+      <c r="A11" s="3">
+        <v>1204</v>
+      </c>
       <c r="B11" s="3" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>9</v>
+        <v>97</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>252</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>10</v>
+        <v>98</v>
       </c>
       <c r="F11" s="3"/>
-      <c r="J11">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <v>1205</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="J12">
         <v>0.05</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
-        <v>2105</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="J12">
-        <v>0.01</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
-        <v>1101</v>
+        <v>2101</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>73</v>
+        <v>4</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>118</v>
+        <v>103</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>108</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>78</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="F13" s="3"/>
       <c r="J13">
         <v>0.01</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
-        <v>4103</v>
+        <v>2101</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>235</v>
+        <v>4</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>34</v>
+        <v>103</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="J14">
-        <v>0.01</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
-        <v>4103</v>
+        <v>2102</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>235</v>
+        <v>69</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>38</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="3"/>
       <c r="J15">
         <v>0.01</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
-        <v>4104</v>
+        <v>2103</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>236</v>
+        <v>70</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>11</v>
+        <v>103</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>32</v>
+        <v>105</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>105</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="J16">
         <v>0.01</v>
@@ -1685,105 +1699,105 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
-        <v>4104</v>
+        <v>2103</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>236</v>
+        <v>70</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E17" s="3"/>
+        <v>103</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>104</v>
+      </c>
       <c r="F17" s="3"/>
       <c r="J17">
         <v>0.01</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
-        <v>4104</v>
+        <v>2104</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>236</v>
+        <v>71</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>36</v>
+        <v>103</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>142</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>65</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="F18" s="3"/>
       <c r="J18">
         <v>0.01</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
-        <v>4105</v>
+        <v>2105</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>158</v>
+        <v>72</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F19" s="3"/>
+        <v>103</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="J19">
         <v>0.01</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
-        <v>4106</v>
+        <v>2106</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>163</v>
+        <v>122</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>128</v>
+        <v>103</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="J20">
         <v>0.01</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="102" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
-        <v>4107</v>
+        <v>2107</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>237</v>
+        <v>141</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>42</v>
+        <v>103</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>140</v>
       </c>
       <c r="F21" s="3"/>
       <c r="J21">
@@ -1792,376 +1806,348 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
-        <v>1201</v>
+        <v>3101</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>73</v>
+        <v>4</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>101</v>
+        <v>31</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>99</v>
+        <v>31</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="J22">
         <v>0.01</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
-        <v>2104</v>
+        <v>3101</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>72</v>
+        <v>4</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>143</v>
+        <v>106</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>29</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F23" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="J23">
         <v>0.01</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
-        <v>1102</v>
+        <v>3102</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>95</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="D24" s="13"/>
+      <c r="E24" s="3"/>
       <c r="F24" s="3"/>
-      <c r="J24">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
-        <v>4108</v>
+        <v>3103</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>238</v>
+        <v>157</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
+        <v>106</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F25" s="11"/>
       <c r="J25">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
-        <v>4109</v>
+        <v>3104</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>65</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="F26" s="3"/>
       <c r="J26">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
-        <v>4109</v>
+        <v>3105</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>73</v>
+        <v>156</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>65</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
       <c r="J27">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
-        <v>4109</v>
+        <v>3106</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>73</v>
+        <v>165</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>65</v>
+        <v>106</v>
       </c>
       <c r="J28">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
-        <v>4109</v>
+        <v>3107</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>73</v>
+        <v>158</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>65</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
       <c r="J29">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
-        <v>3101</v>
+        <v>3108</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="F30" s="3"/>
+        <v>106</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3" t="s">
+        <v>92</v>
+      </c>
       <c r="J30">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
-        <v>4109</v>
+        <v>4101</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>73</v>
+        <v>4</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>25</v>
+      <c r="D31" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>65</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="F31" s="3"/>
       <c r="J31">
         <v>0.01</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
-        <v>2103</v>
+        <v>4101</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>71</v>
+        <v>4</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>89</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F32" s="3"/>
       <c r="J32">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
-        <v>2103</v>
+        <v>4102</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="F33" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="J33">
         <v>0.01</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
-        <v>1103</v>
+        <v>4103</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>71</v>
+        <v>157</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>96</v>
+        <v>11</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>76</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="F34" s="3"/>
       <c r="J34">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
-        <v>3103</v>
+        <v>4104</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>158</v>
+        <v>235</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F35" s="11"/>
+        <v>11</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="J35">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
-        <v>4109</v>
+        <v>4104</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>73</v>
+        <v>235</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>66</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
       <c r="J36">
         <v>0.01</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
-        <v>1202</v>
+        <v>4104</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>71</v>
+        <v>235</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>100</v>
+        <v>11</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>99</v>
+        <v>32</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="J37">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
-        <v>4302</v>
+        <v>4105</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>70</v>
+        <v>234</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D38" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="E38" s="3">
-        <v>1000</v>
+        <v>11</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>77</v>
+        <v>38</v>
       </c>
       <c r="J38">
         <v>0.05</v>
@@ -2169,234 +2155,242 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
-        <v>4203</v>
+        <v>4105</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E39" s="3">
-        <v>6</v>
+        <v>35</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="J39">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="102" x14ac:dyDescent="0.2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
-        <v>2101</v>
+        <v>4106</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="F40" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>127</v>
+      </c>
       <c r="J40">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
-        <v>4303</v>
+        <v>4107</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>12</v>
+        <v>236</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="E41" s="3">
-        <v>1000</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>84</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F41" s="3"/>
       <c r="J41">
         <v>0.05</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
-        <v>4203</v>
+        <v>4108</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3">
-        <v>34</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>49</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
       <c r="J42">
         <v>0.03</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
-        <v>4304</v>
+        <v>4109</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>154</v>
+        <v>72</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D43" s="3">
-        <v>231</v>
+        <v>11</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="F43" s="3"/>
       <c r="J43">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
-        <v>2102</v>
+        <v>4109</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>109</v>
+        <v>11</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F44" s="3"/>
       <c r="J44">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
-        <v>2102</v>
+        <v>4109</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>31</v>
+        <v>11</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="J45">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
-        <v>4204</v>
+        <v>4109</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>243</v>
+        <v>72</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
+        <v>24</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>65</v>
+      </c>
       <c r="J46">
         <v>0.01</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
-        <v>4204</v>
+        <v>4109</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>243</v>
+        <v>72</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3">
-        <v>34</v>
-      </c>
-      <c r="F47" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>65</v>
+      </c>
       <c r="J47">
         <v>0.01</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
-        <v>1104</v>
+        <v>4109</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D48" s="12" t="s">
-        <v>145</v>
+        <v>11</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F48" s="3"/>
+        <v>63</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>65</v>
+      </c>
       <c r="J48">
         <v>0.01</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
-        <v>3104</v>
+        <v>4109</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D49" s="8" t="s">
-        <v>31</v>
+        <v>11</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="J49">
         <v>0.01</v>
@@ -2404,172 +2398,158 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
-        <v>3104</v>
+        <v>4109</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D50" s="13" t="s">
-        <v>29</v>
+        <v>11</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="J50">
         <v>0.01</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
-        <v>4401</v>
+        <v>4110</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C51" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="D51" s="9" t="s">
-        <v>151</v>
+        <v>238</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F51" s="3" t="s">
-        <v>87</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="F51" s="3"/>
       <c r="J51">
         <v>0.01</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
-        <v>4109</v>
+        <v>4111</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>73</v>
+        <v>239</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D52" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F52" s="3" t="s">
-        <v>65</v>
-      </c>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
       <c r="J52">
         <v>0.01</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
-        <v>4109</v>
+        <v>4112</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>73</v>
+        <v>240</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F53" s="3" t="s">
-        <v>65</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
       <c r="J53">
         <v>0.01</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A54" s="3">
-        <v>1203</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D54" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F54" s="3"/>
-      <c r="J54">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A55" s="3">
-        <v>4305</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D55" s="3">
-        <v>12098</v>
-      </c>
-      <c r="E55" s="3" t="s">
+    <row r="54" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="17">
+        <v>4114</v>
+      </c>
+      <c r="B54" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="C54" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="D54" s="17"/>
+      <c r="E54" s="17"/>
+      <c r="F54" s="17"/>
+      <c r="J54" s="18">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="17">
+        <v>4113</v>
+      </c>
+      <c r="B55" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="F55" s="3"/>
-      <c r="J55">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A56" s="3">
-        <v>4205</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D56" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
-      <c r="J56">
+      <c r="C55" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="D55" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="E55" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="F55" s="17"/>
+      <c r="J55" s="18">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="17">
+        <v>4113</v>
+      </c>
+      <c r="B56" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C56" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="D56" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="E56" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="F56" s="17"/>
+      <c r="J56" s="18">
         <v>0.01</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
-        <v>4206</v>
+        <v>4201</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>244</v>
+        <v>4</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E57" s="3">
-        <v>7</v>
+        <v>31</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="F57" s="3"/>
       <c r="J57">
@@ -2578,19 +2558,19 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
-        <v>4110</v>
+        <v>4201</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>239</v>
+        <v>4</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>46</v>
+        <v>5</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="F58" s="3"/>
       <c r="J58">
@@ -2599,100 +2579,106 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
-        <v>4306</v>
+        <v>4202</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>85</v>
+        <v>132</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D59" s="8" t="s">
-        <v>67</v>
+        <v>5</v>
+      </c>
+      <c r="D59" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="E59" s="3">
-        <v>1000</v>
-      </c>
-      <c r="F59" s="3" t="s">
-        <v>86</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="F59" s="3"/>
       <c r="J59">
         <v>0.01</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
-        <v>4111</v>
+        <v>4203</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D60" s="3"/>
-      <c r="E60" s="3"/>
-      <c r="F60" s="3"/>
+        <v>5</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="J60">
         <v>0.01</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
-        <v>4112</v>
+        <v>4203</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="E61" s="3"/>
-      <c r="F61" s="3"/>
+        <v>52</v>
+      </c>
+      <c r="E61" s="3">
+        <v>6</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="J61">
         <v>0.01</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
-        <v>4207</v>
+        <v>4203</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D62" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3">
+        <v>34</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="J62">
         <v>0.01</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
-        <v>4207</v>
+        <v>4204</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E63" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="E63" s="3"/>
       <c r="F63" s="3"/>
       <c r="J63">
         <v>0.01</v>
@@ -2700,19 +2686,17 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="3">
-        <v>4207</v>
+        <v>4204</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D64" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E64" s="3" t="s">
-        <v>55</v>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3">
+        <v>34</v>
       </c>
       <c r="F64" s="3"/>
       <c r="J64">
@@ -2721,15 +2705,17 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
-        <v>4113</v>
+        <v>4205</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>242</v>
+        <v>16</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D65" s="3"/>
+        <v>5</v>
+      </c>
+      <c r="D65" s="11" t="s">
+        <v>23</v>
+      </c>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
       <c r="J65">
@@ -2738,19 +2724,19 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
-        <v>4113</v>
+        <v>4206</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>69</v>
+        <v>243</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>51</v>
+        <v>5</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E66" s="3">
+        <v>7</v>
       </c>
       <c r="F66" s="3"/>
       <c r="J66">
@@ -2759,135 +2745,152 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
-        <v>3107</v>
+        <v>4207</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>166</v>
+        <v>244</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>107</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F67" s="3"/>
       <c r="J67">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
-        <v>3102</v>
+        <v>4207</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>157</v>
+        <v>244</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D68" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="E68" s="3"/>
+        <v>5</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F68" s="3"/>
       <c r="J68">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
-        <v>2106</v>
+        <v>4207</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>123</v>
+        <v>244</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D69" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="E69" s="3"/>
-      <c r="F69" s="3" t="s">
-        <v>90</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F69" s="3"/>
       <c r="J69">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" s="3">
-        <v>1105</v>
+        <v>4208</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>121</v>
+        <v>245</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D70" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="E70" s="3"/>
+        <v>5</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E70" s="3">
+        <v>9</v>
+      </c>
       <c r="F70" s="3"/>
       <c r="J70">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
-        <v>3106</v>
+        <v>4301</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>159</v>
+        <v>4</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D71" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="E71" s="3"/>
-      <c r="F71" s="3"/>
+        <v>21</v>
+      </c>
+      <c r="D71" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>82</v>
+      </c>
       <c r="J71">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" s="3">
-        <v>4208</v>
+        <v>4302</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>246</v>
+        <v>69</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>56</v>
+        <v>21</v>
+      </c>
+      <c r="D72" s="13" t="s">
+        <v>118</v>
       </c>
       <c r="E72" s="3">
-        <v>9</v>
-      </c>
-      <c r="F72" s="3"/>
+        <v>1000</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="J72">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
-        <v>1106</v>
+        <v>4303</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>95</v>
+        <v>21</v>
+      </c>
+      <c r="D73" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="E73" s="3">
+        <v>1000</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="J73">
         <v>0.01</v>
@@ -2895,69 +2898,67 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
-        <v>4402</v>
+        <v>4304</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>70</v>
+        <v>153</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D74" s="5" t="s">
-        <v>120</v>
+        <v>21</v>
+      </c>
+      <c r="D74" s="3">
+        <v>231</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="F74" s="3" t="s">
-        <v>77</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="F74" s="3"/>
       <c r="J74">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
-        <v>4113</v>
+        <v>4305</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>22</v>
+        <v>251</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>59</v>
+        <v>21</v>
+      </c>
+      <c r="D75" s="3">
+        <v>12098</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="F75" s="3"/>
       <c r="J75">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" s="3">
-        <v>1204</v>
+        <v>4306</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>98</v>
+        <v>21</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="E76" s="3" t="s">
-        <v>99</v>
+        <v>66</v>
+      </c>
+      <c r="E76" s="3">
+        <v>1000</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="J76">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.2">
@@ -2977,69 +2978,134 @@
         <v>7</v>
       </c>
       <c r="F77" s="3"/>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A78" s="16" t="s">
-        <v>248</v>
-      </c>
-      <c r="B78" t="s">
-        <v>247</v>
-      </c>
-      <c r="C78" s="3" t="s">
+      <c r="J77">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A78" s="3">
+        <v>4401</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C78" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D78" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F78" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="J78">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A79" s="3">
+        <v>4402</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E79" s="3" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A79" s="16" t="s">
-        <v>249</v>
-      </c>
-      <c r="B79" t="s">
-        <v>158</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>102</v>
+      <c r="F79" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="J79">
+        <v>0.03</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" s="16" t="s">
+        <v>247</v>
+      </c>
+      <c r="B80" t="s">
+        <v>157</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" s="16" t="s">
+        <v>248</v>
+      </c>
+      <c r="B81" t="s">
+        <v>246</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" s="16" t="s">
+        <v>249</v>
+      </c>
+      <c r="B82" t="s">
+        <v>162</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" s="16" t="s">
         <v>250</v>
       </c>
-      <c r="B80" t="s">
-        <v>163</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81" s="16" t="s">
-        <v>251</v>
-      </c>
-      <c r="B81" t="s">
-        <v>73</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A84" s="2" t="s">
-        <v>127</v>
+      <c r="B83" t="s">
+        <v>72</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" s="3"/>
+      <c r="B84" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F84" s="3"/>
+    </row>
+    <row r="87" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A87" s="2" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I81" xr:uid="{E25534D8-8326-A74F-A2E5-C7F409A5D2ED}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:I77">
-      <sortCondition ref="A1:A81"/>
+  <autoFilter ref="A1:I84" xr:uid="{E25534D8-8326-A74F-A2E5-C7F409A5D2ED}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A31:I83">
+      <sortCondition ref="A1:A84"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="D40" r:id="rId1" display="example@gmial.com" xr:uid="{26614BCF-17CC-CC4B-8956-8F6930E60309}"/>
-    <hyperlink ref="E40" r:id="rId2" display="example@gmail.com" xr:uid="{8748665C-4957-DF46-BCAE-78DDC2747FA2}"/>
-    <hyperlink ref="E32" r:id="rId3" xr:uid="{C97D70EF-2237-5345-A311-3AAA5FB2604F}"/>
-    <hyperlink ref="D33" r:id="rId4" xr:uid="{5452BAFC-13C2-3F47-9997-9E87936810D4}"/>
-    <hyperlink ref="E33" r:id="rId5" xr:uid="{26E7AAAB-28B9-3346-B8F0-69E39759EBA8}"/>
-    <hyperlink ref="E12" r:id="rId6" xr:uid="{1E86A40A-BC53-844D-A055-9CA50642AB3B}"/>
+    <hyperlink ref="D21" r:id="rId1" display="example@gmial.com" xr:uid="{26614BCF-17CC-CC4B-8956-8F6930E60309}"/>
+    <hyperlink ref="E21" r:id="rId2" display="example@gmail.com" xr:uid="{8748665C-4957-DF46-BCAE-78DDC2747FA2}"/>
+    <hyperlink ref="E16" r:id="rId3" xr:uid="{C97D70EF-2237-5345-A311-3AAA5FB2604F}"/>
+    <hyperlink ref="D17" r:id="rId4" xr:uid="{5452BAFC-13C2-3F47-9997-9E87936810D4}"/>
+    <hyperlink ref="E17" r:id="rId5" xr:uid="{26E7AAAB-28B9-3346-B8F0-69E39759EBA8}"/>
+    <hyperlink ref="E19" r:id="rId6" xr:uid="{1E86A40A-BC53-844D-A055-9CA50642AB3B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3057,12 +3123,12 @@
   <sheetData>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
@@ -3072,322 +3138,322 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -3421,7 +3487,7 @@
         <v>1101</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -3429,7 +3495,7 @@
         <v>1102</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -3437,7 +3503,7 @@
         <v>1103</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -3453,7 +3519,7 @@
         <v>1105</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -3461,7 +3527,7 @@
         <v>1106</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -3469,7 +3535,7 @@
         <v>1201</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -3477,7 +3543,7 @@
         <v>1202</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -3493,7 +3559,7 @@
         <v>1204</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -3501,7 +3567,7 @@
         <v>2101</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -3517,7 +3583,7 @@
         <v>2103</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -3525,7 +3591,7 @@
         <v>2104</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -3541,7 +3607,7 @@
         <v>2106</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -3549,7 +3615,7 @@
         <v>2107</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -3557,7 +3623,7 @@
         <v>2108</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -3565,7 +3631,7 @@
         <v>3101</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -3573,7 +3639,7 @@
         <v>3102</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -3581,7 +3647,7 @@
         <v>3103</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -3589,7 +3655,7 @@
         <v>3104</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -3613,7 +3679,7 @@
         <v>3107</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -3621,7 +3687,7 @@
         <v>3108</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -3637,7 +3703,7 @@
         <v>4102</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -3645,7 +3711,7 @@
         <v>4103</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -3653,7 +3719,7 @@
         <v>4104</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -3661,7 +3727,7 @@
         <v>4104</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -3669,7 +3735,7 @@
         <v>4104</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -3677,7 +3743,7 @@
         <v>4105</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -3685,7 +3751,7 @@
         <v>4106</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -3709,7 +3775,7 @@
         <v>4109</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -3725,7 +3791,7 @@
         <v>4111</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -3733,7 +3799,7 @@
         <v>4112</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -3741,7 +3807,7 @@
         <v>4113</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -3749,7 +3815,7 @@
         <v>4113</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
@@ -3765,7 +3831,7 @@
         <v>4113</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
@@ -3781,7 +3847,7 @@
         <v>4202</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -3789,7 +3855,7 @@
         <v>4203</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -3797,7 +3863,7 @@
         <v>4203</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -3805,7 +3871,7 @@
         <v>4203</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -3813,7 +3879,7 @@
         <v>4204</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
@@ -3821,7 +3887,7 @@
         <v>4204</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
@@ -3861,7 +3927,7 @@
         <v>4301</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
@@ -3877,7 +3943,7 @@
         <v>4303</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
@@ -3893,7 +3959,7 @@
         <v>4305</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
@@ -3917,7 +3983,7 @@
         <v>4308</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
@@ -3933,7 +3999,7 @@
         <v>4402</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
adrress detection & correction
</commit_message>
<xml_diff>
--- a/src/raw_data/TG_errors.xlsx
+++ b/src/raw_data/TG_errors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tjasagrabnar/Desktop/magistrska/customer_data_cleanup/src/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F54713-F3DD-2042-888F-24CBB9BE2436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE4F0DE4-3B6E-624C-BC88-88E537A2B392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17160" yWindow="1020" windowWidth="16880" windowHeight="21080" xr2:uid="{AE53E973-26AC-D344-B98A-BA50389E6E12}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="34200" windowHeight="21380" xr2:uid="{AE53E973-26AC-D344-B98A-BA50389E6E12}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$1:$I$84</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$1:$J$81</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="249">
   <si>
     <t>Error_ID</t>
   </si>
@@ -196,9 +196,6 @@
     <t>A</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>BŠ 6</t>
   </si>
   <si>
@@ -220,9 +217,6 @@
     <t>6/B</t>
   </si>
   <si>
-    <t>Ellerjeva 39</t>
-  </si>
-  <si>
     <t>Trg izgnancev</t>
   </si>
   <si>
@@ -385,13 +379,7 @@
     <t>Correction</t>
   </si>
   <si>
-    <t>STREET_NAME and HOUSE_NUMBER</t>
-  </si>
-  <si>
     <t>street name foreign address but have slovenia as country</t>
-  </si>
-  <si>
-    <t>STREET_NAME and COUNTRY</t>
   </si>
   <si>
     <t>John John</t>
@@ -788,9 +776,6 @@
     <t>Cannot contain digit at the end</t>
   </si>
   <si>
-    <t>Street name foreign address but have slovenia as country</t>
-  </si>
-  <si>
     <t>No house number</t>
   </si>
   <si>
@@ -822,13 +807,16 @@
   </si>
   <si>
     <t>DOE</t>
+  </si>
+  <si>
+    <t>ERROR_MESSAGE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -881,19 +869,12 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF9C0006"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -903,11 +884,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -935,13 +911,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
@@ -984,14 +959,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="Bad" xfId="3" builtinId="27"/>
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="1" builtinId="10"/>
@@ -1326,11 +1296,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E25534D8-8326-A74F-A2E5-C7F409A5D2ED}">
-  <dimension ref="A1:J87"/>
+  <dimension ref="A1:M84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A55" sqref="A55"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M31" sqref="M31:M80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1338,47 +1308,51 @@
     <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.33203125" customWidth="1"/>
     <col min="3" max="3" width="31.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.6640625" customWidth="1"/>
-    <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.1640625" customWidth="1"/>
+    <col min="5" max="5" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.6640625" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="J1" s="15" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="J1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1101</v>
       </c>
@@ -1386,129 +1360,177 @@
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="E2" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" s="3" t="str">
+        <f>_xlfn.CONCAT(C2,": ", B2)</f>
+        <v>NAME: Missing Data</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="J2">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G2" s="3"/>
+      <c r="K2">
+        <v>0.01</v>
+      </c>
+      <c r="M2" t="str">
+        <f>_xlfn.CONCAT("'",A2,"': '",D2,"',")</f>
+        <v>'1101': 'NAME: Missing Data',</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>1102</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>110</v>
+        <v>91</v>
+      </c>
+      <c r="D3" s="3" t="str">
+        <f t="shared" ref="D3:D66" si="0">_xlfn.CONCAT(C3,": ", B3)</f>
+        <v>NAME: Unnecessary Spaces</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="J3">
+        <v>92</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="K3">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M3" t="str">
+        <f t="shared" ref="M3:M66" si="1">_xlfn.CONCAT("'",A3,"': '",D3,"',")</f>
+        <v>'1102': 'NAME: Unnecessary Spaces',</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>1103</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>NAME: Invalid Characters</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>94</v>
-      </c>
       <c r="F4" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="J4">
+        <v>92</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="K4">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="M4" t="str">
+        <f t="shared" si="1"/>
+        <v>'1103': 'NAME: Invalid Characters',</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>1104</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="E5" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>NAME: Formatting Issue</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="F5" s="3"/>
-      <c r="J5">
+      <c r="F5" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="K5">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M5" t="str">
+        <f t="shared" si="1"/>
+        <v>'1104': 'NAME: Formatting Issue',</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>1105</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
+      </c>
+      <c r="D6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>NAME: Duplicates</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>113</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="J6">
+        <v>92</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="K6">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M6" t="str">
+        <f t="shared" si="1"/>
+        <v>'1105': 'NAME: Duplicates',</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>1106</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="E7" s="3"/>
+        <v>91</v>
+      </c>
+      <c r="D7" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>NAME: Two names in one field</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>117</v>
+      </c>
       <c r="F7" s="3"/>
-      <c r="J7">
+      <c r="G7" s="3"/>
+      <c r="K7">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="M7" t="str">
+        <f t="shared" si="1"/>
+        <v>'1106': 'NAME: Two names in one field',</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>1201</v>
       </c>
@@ -1516,107 +1538,147 @@
         <v>4</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="E8" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>SURNAME: Missing Data</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="3"/>
-      <c r="J8">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G8" s="3"/>
+      <c r="K8">
+        <v>0.01</v>
+      </c>
+      <c r="M8" t="str">
+        <f t="shared" si="1"/>
+        <v>'1201': 'SURNAME: Missing Data',</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>1202</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
+      </c>
+      <c r="D9" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>SURNAME: Unnecessary Spaces</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>107</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="J9">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="K9">
+        <v>0.01</v>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" si="1"/>
+        <v>'1202': 'SURNAME: Unnecessary Spaces',</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>1203</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>SURNAME: Invalid Characters</v>
+      </c>
+      <c r="E10" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>98</v>
-      </c>
       <c r="F10" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="J10">
+        <v>96</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="K10">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M10" t="str">
+        <f t="shared" si="1"/>
+        <v>'1203': 'SURNAME: Invalid Characters',</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>1204</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>252</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+      <c r="D11" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>SURNAME: Formatting Issue</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="M11" t="str">
+        <f t="shared" si="1"/>
+        <v>'1204': 'SURNAME: Formatting Issue',</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>1205</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="E12" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>SURNAME: Duplicates</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>98</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="J12">
+        <v>96</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="K12">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M12" t="str">
+        <f t="shared" si="1"/>
+        <v>'1205': 'SURNAME: Duplicates',</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>2101</v>
       </c>
@@ -1624,20 +1686,28 @@
         <v>4</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="E13" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D13" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>EMAIL: Missing Data</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F13" s="3"/>
-      <c r="J13">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G13" s="3"/>
+      <c r="K13">
+        <v>0.01</v>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" si="1"/>
+        <v>'2101': 'EMAIL: Missing Data',</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>2101</v>
       </c>
@@ -1645,166 +1715,230 @@
         <v>4</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D14" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D14" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>EMAIL: Missing Data</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="F14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G14" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="M14" t="str">
+        <f t="shared" si="1"/>
+        <v>'2101': 'EMAIL: Missing Data',</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>2102</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D15" s="4"/>
+        <v>101</v>
+      </c>
+      <c r="D15" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>EMAIL: Unnecessary Spaces</v>
+      </c>
       <c r="E15" s="4"/>
-      <c r="F15" s="3"/>
-      <c r="J15">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F15" s="4"/>
+      <c r="G15" s="3"/>
+      <c r="K15">
+        <v>0.01</v>
+      </c>
+      <c r="M15" t="str">
+        <f t="shared" si="1"/>
+        <v>'2102': 'EMAIL: Unnecessary Spaces',</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>2103</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D16" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>EMAIL: Invalid Characters</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="J16">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F16" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="K16">
+        <v>0.01</v>
+      </c>
+      <c r="M16" t="str">
+        <f t="shared" si="1"/>
+        <v>'2103': 'EMAIL: Invalid Characters',</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>2103</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D17" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>EMAIL: Invalid Characters</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="F17" s="3"/>
-      <c r="J17">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="F17" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G17" s="3"/>
+      <c r="K17">
+        <v>0.01</v>
+      </c>
+      <c r="M17" t="str">
+        <f t="shared" si="1"/>
+        <v>'2103': 'EMAIL: Invalid Characters',</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>2104</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="F18" s="3"/>
-      <c r="J18">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+      <c r="D18" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>EMAIL: Formatting Issue</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G18" s="3"/>
+      <c r="K18">
+        <v>0.01</v>
+      </c>
+      <c r="M18" t="str">
+        <f t="shared" si="1"/>
+        <v>'2104': 'EMAIL: Formatting Issue',</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>2105</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="J19">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+      <c r="D19" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>EMAIL: Duplicates</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="K19">
+        <v>0.01</v>
+      </c>
+      <c r="M19" t="str">
+        <f t="shared" si="1"/>
+        <v>'2105': 'EMAIL: Duplicates',</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>2106</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="J20">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="102" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+      <c r="D20" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>EMAIL: Two Emails</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="K20">
+        <v>0.01</v>
+      </c>
+      <c r="M20" t="str">
+        <f t="shared" si="1"/>
+        <v>'2106': 'EMAIL: Two Emails',</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="102" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>2107</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>139</v>
+        <v>101</v>
+      </c>
+      <c r="D21" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>EMAIL: Invalid domain</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="F21" s="3"/>
-      <c r="J21">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="G21" s="3"/>
+      <c r="K21">
+        <v>0.01</v>
+      </c>
+      <c r="M21" t="str">
+        <f t="shared" si="1"/>
+        <v>'2107': 'EMAIL: Invalid domain',</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>3101</v>
       </c>
@@ -1812,22 +1946,30 @@
         <v>4</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D22" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D22" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PHONE: Missing Data</v>
+      </c>
+      <c r="E22" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="F22" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F22" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="J22">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G22" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="K22">
+        <v>0.01</v>
+      </c>
+      <c r="M22" t="str">
+        <f t="shared" si="1"/>
+        <v>'3101': 'PHONE: Missing Data',</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>3101</v>
       </c>
@@ -1835,151 +1977,215 @@
         <v>4</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D23" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="D23" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PHONE: Missing Data</v>
+      </c>
+      <c r="E23" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="F23" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F23" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="J23">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G23" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="K23">
+        <v>0.01</v>
+      </c>
+      <c r="M23" t="str">
+        <f t="shared" si="1"/>
+        <v>'3101': 'PHONE: Missing Data',</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>3102</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D24" s="13"/>
-      <c r="E24" s="3"/>
+        <v>104</v>
+      </c>
+      <c r="D24" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PHONE: Unnecessary Spaces</v>
+      </c>
+      <c r="E24" s="13"/>
       <c r="F24" s="3"/>
-    </row>
-    <row r="25" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="G24" s="3"/>
+      <c r="M24" t="str">
+        <f t="shared" si="1"/>
+        <v>'3102': 'PHONE: Unnecessary Spaces',</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>3103</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="F25" s="11"/>
-      <c r="J25">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+      <c r="D25" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PHONE: Invalid characters</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="G25" s="11"/>
+      <c r="K25">
+        <v>0.01</v>
+      </c>
+      <c r="M25" t="str">
+        <f t="shared" si="1"/>
+        <v>'3103': 'PHONE: Invalid characters',</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>3104</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D26" s="12" t="s">
-        <v>145</v>
+        <v>104</v>
+      </c>
+      <c r="D26" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PHONE: Formatting Issue</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="F26" s="3"/>
-      <c r="J26">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="G26" s="3"/>
+      <c r="K26">
+        <v>0.01</v>
+      </c>
+      <c r="M26" t="str">
+        <f t="shared" si="1"/>
+        <v>'3104': 'PHONE: Formatting Issue',</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>3105</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="E27" s="3"/>
+        <v>104</v>
+      </c>
+      <c r="D27" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PHONE: Too many digits</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>143</v>
+      </c>
       <c r="F27" s="3"/>
-      <c r="J27">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G27" s="3"/>
+      <c r="K27">
+        <v>0.01</v>
+      </c>
+      <c r="M27" t="str">
+        <f t="shared" si="1"/>
+        <v>'3105': 'PHONE: Too many digits',</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>3106</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="J28">
+        <v>104</v>
+      </c>
+      <c r="D28" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PHONE: Too little digits</v>
+      </c>
+      <c r="K28">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M28" t="str">
+        <f t="shared" si="1"/>
+        <v>'3106': 'PHONE: Too little digits',</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>3107</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="E29" s="3"/>
+        <v>104</v>
+      </c>
+      <c r="D29" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PHONE: Two phone numbers</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>119</v>
+      </c>
       <c r="F29" s="3"/>
-      <c r="J29">
+      <c r="G29" s="3"/>
+      <c r="K29">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M29" t="str">
+        <f t="shared" si="1"/>
+        <v>'3107': 'PHONE: Two phone numbers',</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>3108</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="J30">
+        <v>104</v>
+      </c>
+      <c r="D30" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PHONE: Different country format</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="K30">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M30" t="str">
+        <f t="shared" si="1"/>
+        <v>'3108': 'PHONE: Different country format',</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>4101</v>
       </c>
@@ -1989,18 +2195,26 @@
       <c r="C31" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>STREET_NAME: Missing Data</v>
+      </c>
+      <c r="E31" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="F31" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F31" s="3"/>
-      <c r="J31">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G31" s="3"/>
+      <c r="K31">
+        <v>0.01</v>
+      </c>
+      <c r="M31" t="str">
+        <f t="shared" si="1"/>
+        <v>'4101': 'STREET_NAME: Missing Data',</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>4101</v>
       </c>
@@ -2010,1104 +2224,1446 @@
       <c r="C32" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>STREET_NAME: Missing Data</v>
+      </c>
+      <c r="E32" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="F32" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F32" s="3"/>
-      <c r="J32">
+      <c r="G32" s="3"/>
+      <c r="K32">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M32" t="str">
+        <f t="shared" si="1"/>
+        <v>'4101': 'STREET_NAME: Missing Data',</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>4102</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>STREET_NAME: Unnecessary Spaces</v>
+      </c>
+      <c r="E33" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="F33" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F33" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="J33">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G33" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="K33">
+        <v>0.01</v>
+      </c>
+      <c r="M33" t="str">
+        <f t="shared" si="1"/>
+        <v>'4102': 'STREET_NAME: Unnecessary Spaces',</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>4103</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>STREET_NAME: Invalid characters</v>
+      </c>
+      <c r="E34" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="F34" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F34" s="3"/>
-      <c r="J34">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G34" s="3"/>
+      <c r="K34">
+        <v>0.01</v>
+      </c>
+      <c r="M34" t="str">
+        <f t="shared" si="1"/>
+        <v>'4103': 'STREET_NAME: Invalid characters',</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>4104</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>STREET_NAME: Contains house number</v>
+      </c>
+      <c r="E35" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="F35" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F35" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="J35">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G35" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="K35">
+        <v>0.01</v>
+      </c>
+      <c r="M35" t="str">
+        <f t="shared" si="1"/>
+        <v>'4104': 'STREET_NAME: Contains house number',</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>4104</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D36" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>STREET_NAME: Contains house number</v>
+      </c>
+      <c r="E36" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E36" s="3"/>
       <c r="F36" s="3"/>
-      <c r="J36">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G36" s="3"/>
+      <c r="K36">
+        <v>0.01</v>
+      </c>
+      <c r="M36" t="str">
+        <f t="shared" si="1"/>
+        <v>'4104': 'STREET_NAME: Contains house number',</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>4104</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D37" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>STREET_NAME: Contains house number</v>
+      </c>
+      <c r="E37" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="F37" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F37" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="J37">
+      <c r="G37" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="K37">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M37" t="str">
+        <f t="shared" si="1"/>
+        <v>'4104': 'STREET_NAME: Contains house number',</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>4105</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D38" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>STREET_NAME: Contains variation of BŠ</v>
+      </c>
+      <c r="E38" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="F38" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="G38" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="J38">
+      <c r="K38">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M38" t="str">
+        <f t="shared" si="1"/>
+        <v>'4105': 'STREET_NAME: Contains variation of BŠ',</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>4105</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D39" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>STREET_NAME: Contains variation of BŠ</v>
+      </c>
+      <c r="E39" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="F39" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F39" s="3" t="s">
+      <c r="G39" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="J39">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+      <c r="K39">
+        <v>0.01</v>
+      </c>
+      <c r="M39" t="str">
+        <f t="shared" si="1"/>
+        <v>'4105': 'STREET_NAME: Contains variation of BŠ',</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>4106</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D40" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>STREET_NAME: Invalid abbreviations</v>
+      </c>
+      <c r="E40" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E40" s="3" t="s">
+      <c r="F40" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F40" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="J40">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G40" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="K40">
+        <v>0.01</v>
+      </c>
+      <c r="M40" t="str">
+        <f t="shared" si="1"/>
+        <v>'4106': 'STREET_NAME: Invalid abbreviations',</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>4107</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D41" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>STREET_NAME: No space after full stop</v>
+      </c>
+      <c r="E41" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="F41" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F41" s="3"/>
-      <c r="J41">
+      <c r="G41" s="3"/>
+      <c r="K41">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M41" t="str">
+        <f t="shared" si="1"/>
+        <v>'4107': 'STREET_NAME: No space after full stop',</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>4108</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D42" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="E42" s="3"/>
+      <c r="D42" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>STREET_NAME: Only numbers</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>124</v>
+      </c>
       <c r="F42" s="3"/>
-      <c r="J42">
+      <c r="G42" s="3"/>
+      <c r="K42">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M42" t="str">
+        <f t="shared" si="1"/>
+        <v>'4108': 'STREET_NAME: Only numbers',</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>4109</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D43" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>STREET_NAME: Duplicates</v>
+      </c>
+      <c r="E43" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="F43" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F43" s="3"/>
-      <c r="J43">
+      <c r="G43" s="3"/>
+      <c r="K43">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M43" t="str">
+        <f t="shared" si="1"/>
+        <v>'4109': 'STREET_NAME: Duplicates',</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>4109</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D44" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>STREET_NAME: Duplicates</v>
+      </c>
+      <c r="E44" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="F44" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F44" s="3"/>
-      <c r="J44">
+      <c r="G44" s="3"/>
+      <c r="K44">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M44" t="str">
+        <f t="shared" si="1"/>
+        <v>'4109': 'STREET_NAME: Duplicates',</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>4109</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D45" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>STREET_NAME: Duplicates</v>
+      </c>
+      <c r="E45" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E45" s="3" t="s">
+      <c r="F45" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F45" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="J45">
+      <c r="G45" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="K45">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M45" t="str">
+        <f t="shared" si="1"/>
+        <v>'4109': 'STREET_NAME: Duplicates',</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>4109</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="D46" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>STREET_NAME: Duplicates</v>
+      </c>
+      <c r="E46" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E46" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="F46" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="J46">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="K46">
+        <v>0.01</v>
+      </c>
+      <c r="M46" t="str">
+        <f t="shared" si="1"/>
+        <v>'4109': 'STREET_NAME: Duplicates',</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>4109</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="D47" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>STREET_NAME: Duplicates</v>
+      </c>
+      <c r="E47" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E47" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="F47" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="J47">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="K47">
+        <v>0.01</v>
+      </c>
+      <c r="M47" t="str">
+        <f t="shared" si="1"/>
+        <v>'4109': 'STREET_NAME: Duplicates',</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>4109</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D48" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>STREET_NAME: Duplicates</v>
+      </c>
+      <c r="E48" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E48" s="3" t="s">
+      <c r="F48" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G48" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F48" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="J48">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K48">
+        <v>0.01</v>
+      </c>
+      <c r="M48" t="str">
+        <f t="shared" si="1"/>
+        <v>'4109': 'STREET_NAME: Duplicates',</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>4109</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D49" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>STREET_NAME: Duplicates</v>
+      </c>
+      <c r="E49" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E49" s="3" t="s">
-        <v>64</v>
-      </c>
       <c r="F49" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="J49">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="K49">
+        <v>0.01</v>
+      </c>
+      <c r="M49" t="str">
+        <f t="shared" si="1"/>
+        <v>'4109': 'STREET_NAME: Duplicates',</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>4109</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="D50" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>STREET_NAME: Duplicates</v>
+      </c>
+      <c r="E50" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E50" s="3" t="s">
-        <v>60</v>
-      </c>
       <c r="F50" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="J50">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="K50">
+        <v>0.01</v>
+      </c>
+      <c r="M50" t="str">
+        <f t="shared" si="1"/>
+        <v>'4109': 'STREET_NAME: Duplicates',</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>4110</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="D51" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>STREET_NAME: Starts with number</v>
+      </c>
+      <c r="E51" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E51" s="3" t="s">
+      <c r="F51" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F51" s="3"/>
-      <c r="J51">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G51" s="3"/>
+      <c r="K51">
+        <v>0.01</v>
+      </c>
+      <c r="M51" t="str">
+        <f t="shared" si="1"/>
+        <v>'4110': 'STREET_NAME: Starts with number',</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>4111</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D52" s="3"/>
+      <c r="D52" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>STREET_NAME: More than 2 commas</v>
+      </c>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
-      <c r="J52">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G52" s="3"/>
+      <c r="K52">
+        <v>0.01</v>
+      </c>
+      <c r="M52" t="str">
+        <f t="shared" si="1"/>
+        <v>'4111': 'STREET_NAME: More than 2 commas',</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>4112</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D53" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="E53" s="3"/>
+      <c r="D53" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>STREET_NAME: Cannot contain digit at the end</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="F53" s="3"/>
-      <c r="J53">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="17">
-        <v>4114</v>
-      </c>
-      <c r="B54" s="17" t="s">
-        <v>241</v>
-      </c>
-      <c r="C54" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="D54" s="17"/>
-      <c r="E54" s="17"/>
-      <c r="F54" s="17"/>
-      <c r="J54" s="18">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="17">
-        <v>4113</v>
-      </c>
-      <c r="B55" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="C55" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="D55" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="E55" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="F55" s="17"/>
-      <c r="J55" s="18">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="17">
-        <v>4113</v>
-      </c>
-      <c r="B56" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C56" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="D56" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="E56" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="F56" s="17"/>
-      <c r="J56" s="18">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G53" s="3"/>
+      <c r="K53">
+        <v>0.01</v>
+      </c>
+      <c r="M53" t="str">
+        <f t="shared" si="1"/>
+        <v>'4112': 'STREET_NAME: Cannot contain digit at the end',</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A54" s="3">
+        <v>4201</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D54" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>HOUSE_NUMBER: Missing Data</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G54" s="3"/>
+      <c r="K54">
+        <v>0.01</v>
+      </c>
+      <c r="M54" t="str">
+        <f t="shared" si="1"/>
+        <v>'4201': 'HOUSE_NUMBER: Missing Data',</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A55" s="3">
+        <v>4201</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D55" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>HOUSE_NUMBER: Missing Data</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G55" s="3"/>
+      <c r="K55">
+        <v>0.01</v>
+      </c>
+      <c r="M55" t="str">
+        <f t="shared" si="1"/>
+        <v>'4201': 'HOUSE_NUMBER: Missing Data',</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A56" s="3">
+        <v>4202</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D56" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>HOUSE_NUMBER: Unnecessary spaces</v>
+      </c>
+      <c r="E56" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F56" s="3">
+        <v>2</v>
+      </c>
+      <c r="G56" s="3"/>
+      <c r="K56">
+        <v>0.01</v>
+      </c>
+      <c r="M56" t="str">
+        <f t="shared" si="1"/>
+        <v>'4202': 'HOUSE_NUMBER: Unnecessary spaces',</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
-        <v>4201</v>
+        <v>4203</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>4</v>
+        <v>230</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D57" s="5" t="s">
+      <c r="D57" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>HOUSE_NUMBER: Contains variation of BŠ</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F57" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E57" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F57" s="3"/>
-      <c r="J57">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G57" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K57">
+        <v>0.01</v>
+      </c>
+      <c r="M57" t="str">
+        <f t="shared" si="1"/>
+        <v>'4203': 'HOUSE_NUMBER: Contains variation of BŠ',</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
-        <v>4201</v>
+        <v>4203</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>4</v>
+        <v>230</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D58" s="5" t="s">
-        <v>30</v>
+      <c r="D58" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>HOUSE_NUMBER: Contains variation of BŠ</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F58" s="3"/>
-      <c r="J58">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="F58" s="3">
+        <v>6</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="K58">
+        <v>0.01</v>
+      </c>
+      <c r="M58" t="str">
+        <f t="shared" si="1"/>
+        <v>'4203': 'HOUSE_NUMBER: Contains variation of BŠ',</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
-        <v>4202</v>
+        <v>4203</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>132</v>
+        <v>230</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D59" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E59" s="3">
-        <v>2</v>
-      </c>
-      <c r="F59" s="3"/>
-      <c r="J59">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D59" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>HOUSE_NUMBER: Contains variation of BŠ</v>
+      </c>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3">
+        <v>34</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="K59">
+        <v>0.01</v>
+      </c>
+      <c r="M59" t="str">
+        <f t="shared" si="1"/>
+        <v>'4203': 'HOUSE_NUMBER: Contains variation of BŠ',</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
-        <v>4203</v>
+        <v>4204</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D60" s="3" t="s">
-        <v>48</v>
+      <c r="D60" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>HOUSE_NUMBER: No house number</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F60" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="J60">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3"/>
+      <c r="K60">
+        <v>0.01</v>
+      </c>
+      <c r="M60" t="str">
+        <f t="shared" si="1"/>
+        <v>'4204': 'HOUSE_NUMBER: No house number',</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
-        <v>4203</v>
+        <v>4204</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D61" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E61" s="3">
-        <v>6</v>
-      </c>
-      <c r="F61" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="J61">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D61" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>HOUSE_NUMBER: No house number</v>
+      </c>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3">
+        <v>34</v>
+      </c>
+      <c r="G61" s="3"/>
+      <c r="K61">
+        <v>0.01</v>
+      </c>
+      <c r="M61" t="str">
+        <f t="shared" si="1"/>
+        <v>'4204': 'HOUSE_NUMBER: No house number',</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
-        <v>4203</v>
+        <v>4205</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>234</v>
+        <v>16</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D62" s="3"/>
-      <c r="E62" s="3">
-        <v>34</v>
-      </c>
-      <c r="F62" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="J62">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D62" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>HOUSE_NUMBER: invalid combination</v>
+      </c>
+      <c r="E62" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F62" s="3"/>
+      <c r="G62" s="3"/>
+      <c r="K62">
+        <v>0.01</v>
+      </c>
+      <c r="M62" t="str">
+        <f t="shared" si="1"/>
+        <v>'4205': 'HOUSE_NUMBER: invalid combination',</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
-        <v>4204</v>
+        <v>4206</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D63" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
-      <c r="J63">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D63" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>HOUSE_NUMBER: Leading 0</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F63" s="3">
+        <v>7</v>
+      </c>
+      <c r="G63" s="3"/>
+      <c r="K63">
+        <v>0.01</v>
+      </c>
+      <c r="M63" t="str">
+        <f t="shared" si="1"/>
+        <v>'4206': 'HOUSE_NUMBER: Leading 0',</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" s="3">
-        <v>4204</v>
+        <v>4207</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D64" s="3"/>
-      <c r="E64" s="3">
-        <v>34</v>
-      </c>
-      <c r="F64" s="3"/>
-      <c r="J64">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D64" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>HOUSE_NUMBER: Spacing between components</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G64" s="3"/>
+      <c r="K64">
+        <v>0.01</v>
+      </c>
+      <c r="M64" t="str">
+        <f t="shared" si="1"/>
+        <v>'4207': 'HOUSE_NUMBER: Spacing between components',</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
-        <v>4205</v>
+        <v>4207</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>16</v>
+        <v>239</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D65" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E65" s="3"/>
-      <c r="F65" s="3"/>
-      <c r="J65">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D65" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>HOUSE_NUMBER: Spacing between components</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G65" s="3"/>
+      <c r="K65">
+        <v>0.01</v>
+      </c>
+      <c r="M65" t="str">
+        <f t="shared" si="1"/>
+        <v>'4207': 'HOUSE_NUMBER: Spacing between components',</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
-        <v>4206</v>
+        <v>4207</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D66" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E66" s="3">
-        <v>7</v>
-      </c>
-      <c r="F66" s="3"/>
-      <c r="J66">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D66" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>HOUSE_NUMBER: Spacing between components</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G66" s="3"/>
+      <c r="K66">
+        <v>0.01</v>
+      </c>
+      <c r="M66" t="str">
+        <f t="shared" si="1"/>
+        <v>'4207': 'HOUSE_NUMBER: Spacing between components',</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
-        <v>4207</v>
+        <v>4208</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D67" s="3" t="s">
-        <v>54</v>
+      <c r="D67" s="3" t="str">
+        <f t="shared" ref="D67:D81" si="2">_xlfn.CONCAT(C67,": ", B67)</f>
+        <v>HOUSE_NUMBER: Contains roman numerals</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F67" s="3"/>
-      <c r="J67">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F67" s="3">
+        <v>9</v>
+      </c>
+      <c r="G67" s="3"/>
+      <c r="K67">
+        <v>0.02</v>
+      </c>
+      <c r="M67" t="str">
+        <f t="shared" ref="M67:M81" si="3">_xlfn.CONCAT("'",A67,"': '",D67,"',")</f>
+        <v>'4208': 'HOUSE_NUMBER: Contains roman numerals',</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
-        <v>4207</v>
+        <v>4301</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>244</v>
+        <v>4</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F68" s="3"/>
-      <c r="J68">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="D68" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>ZIPCODE: Missing Data</v>
+      </c>
+      <c r="E68" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="K68">
+        <v>0.05</v>
+      </c>
+      <c r="M68" t="str">
+        <f t="shared" si="3"/>
+        <v>'4301': 'ZIPCODE: Missing Data',</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
-        <v>4207</v>
+        <v>4302</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>244</v>
+        <v>67</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F69" s="3"/>
-      <c r="J69">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="D69" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>ZIPCODE: Unnecessary Spaces</v>
+      </c>
+      <c r="E69" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="F69" s="3">
+        <v>1000</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="K69">
+        <v>0.03</v>
+      </c>
+      <c r="M69" t="str">
+        <f t="shared" si="3"/>
+        <v>'4302': 'ZIPCODE: Unnecessary Spaces',</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A70" s="3">
-        <v>4208</v>
+        <v>4303</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>245</v>
+        <v>12</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E70" s="3">
-        <v>9</v>
-      </c>
-      <c r="F70" s="3"/>
-      <c r="J70">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="D70" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>ZIPCODE: invalid characters</v>
+      </c>
+      <c r="E70" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="F70" s="3">
+        <v>1000</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="K70">
+        <v>0.01</v>
+      </c>
+      <c r="M70" t="str">
+        <f t="shared" si="3"/>
+        <v>'4303': 'ZIPCODE: invalid characters',</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
-        <v>4301</v>
+        <v>4304</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>4</v>
+        <v>149</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D71" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>31</v>
+      <c r="D71" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>ZIPCODE: Less than 4</v>
+      </c>
+      <c r="E71" s="3">
+        <v>231</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="J71">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+      <c r="G71" s="3"/>
+      <c r="K71">
+        <v>0.01</v>
+      </c>
+      <c r="M71" t="str">
+        <f t="shared" si="3"/>
+        <v>'4304': 'ZIPCODE: Less than 4',</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72" s="3">
-        <v>4302</v>
+        <v>4305</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>69</v>
+        <v>246</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D72" s="13" t="s">
-        <v>118</v>
+      <c r="D72" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>ZIPCODE: More than 4</v>
       </c>
       <c r="E72" s="3">
-        <v>1000</v>
+        <v>12098</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="J72">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+      <c r="G72" s="3"/>
+      <c r="K72">
+        <v>0.02</v>
+      </c>
+      <c r="M72" t="str">
+        <f t="shared" si="3"/>
+        <v>'4305': 'ZIPCODE: More than 4',</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
-        <v>4303</v>
+        <v>4306</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>12</v>
+        <v>82</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D73" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="E73" s="3">
+      <c r="D73" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>ZIPCODE: Contains Letters</v>
+      </c>
+      <c r="E73" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F73" s="3">
         <v>1000</v>
       </c>
-      <c r="F73" s="3" t="s">
+      <c r="G73" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="J73">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K73">
+        <v>0.01</v>
+      </c>
+      <c r="M73" t="str">
+        <f t="shared" si="3"/>
+        <v>'4306': 'ZIPCODE: Contains Letters',</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
-        <v>4304</v>
+        <v>4307</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>153</v>
+        <v>6</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D74" s="3">
-        <v>231</v>
-      </c>
-      <c r="E74" s="3" t="s">
+      <c r="D74" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>ZIPCODE: Invalid Value</v>
+      </c>
+      <c r="E74" s="3">
+        <v>1000</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G74" s="3"/>
+      <c r="K74">
+        <v>0.05</v>
+      </c>
+      <c r="M74" t="str">
+        <f t="shared" si="3"/>
+        <v>'4307': 'ZIPCODE: Invalid Value',</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A75" s="3">
+        <v>4401</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C75" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="D75" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>POSTAL_CITY: Missing Data</v>
+      </c>
+      <c r="E75" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G75" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K75">
+        <v>0.01</v>
+      </c>
+      <c r="M75" t="str">
+        <f t="shared" si="3"/>
+        <v>'4401': 'POSTAL_CITY: Missing Data',</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A76" s="3">
+        <v>4402</v>
+      </c>
+      <c r="B76" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F74" s="3"/>
-      <c r="J74">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A75" s="3">
-        <v>4305</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D75" s="3">
-        <v>12098</v>
-      </c>
-      <c r="E75" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F75" s="3"/>
-      <c r="J75">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A76" s="3">
-        <v>4306</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>84</v>
-      </c>
       <c r="C76" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D76" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="E76" s="3">
-        <v>1000</v>
+        <v>99</v>
+      </c>
+      <c r="D76" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>POSTAL_CITY: Unnecessary Spaces</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>115</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="J76">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A77" s="3">
-        <v>4307</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>6</v>
+        <v>100</v>
+      </c>
+      <c r="G76" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="K76">
+        <v>0.03</v>
+      </c>
+      <c r="M76" t="str">
+        <f t="shared" si="3"/>
+        <v>'4402': 'POSTAL_CITY: Unnecessary Spaces',</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A77" s="16" t="s">
+        <v>242</v>
+      </c>
+      <c r="B77" t="s">
+        <v>153</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D77" s="3">
-        <v>1000</v>
-      </c>
-      <c r="E77" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F77" s="3"/>
-      <c r="J77">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A78" s="3">
-        <v>4401</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C78" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="D78" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="E78" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F78" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="J78">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A79" s="3">
-        <v>4402</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>69</v>
+        <v>99</v>
+      </c>
+      <c r="D77" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>POSTAL_CITY: Invalid characters</v>
+      </c>
+      <c r="M77" t="str">
+        <f t="shared" si="3"/>
+        <v>'4403': 'POSTAL_CITY: Invalid characters',</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A78" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="B78" t="s">
+        <v>241</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D78" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>POSTAL_CITY: Contains digits</v>
+      </c>
+      <c r="M78" t="str">
+        <f t="shared" si="3"/>
+        <v>'4404': 'POSTAL_CITY: Contains digits',</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A79" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="B79" t="s">
+        <v>158</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D79" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="E79" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="F79" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="J79">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+      <c r="D79" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>POSTAL_CITY: Invalid abbreviations</v>
+      </c>
+      <c r="M79" t="str">
+        <f t="shared" si="3"/>
+        <v>'4405': 'POSTAL_CITY: Invalid abbreviations',</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80" s="16" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B80" t="s">
-        <v>157</v>
+        <v>70</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A81" s="16" t="s">
-        <v>248</v>
-      </c>
-      <c r="B81" t="s">
-        <v>246</v>
+        <v>99</v>
+      </c>
+      <c r="D80" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>POSTAL_CITY: Duplicates</v>
+      </c>
+      <c r="M80" t="str">
+        <f t="shared" si="3"/>
+        <v>'4406': 'POSTAL_CITY: Duplicates',</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A81" s="3"/>
+      <c r="B81" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A82" s="16" t="s">
-        <v>249</v>
-      </c>
-      <c r="B82" t="s">
-        <v>162</v>
-      </c>
-      <c r="C82" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A83" s="16" t="s">
-        <v>250</v>
-      </c>
-      <c r="B83" t="s">
-        <v>72</v>
-      </c>
-      <c r="C83" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A84" s="3"/>
-      <c r="B84" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="D84" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D81" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>NONE: Duplicate Row</v>
+      </c>
+      <c r="E81" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E84" s="3" t="s">
+      <c r="F81" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F84" s="3"/>
-    </row>
-    <row r="87" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A87" s="2" t="s">
-        <v>126</v>
+      <c r="G81" s="3"/>
+      <c r="M81" t="str">
+        <f t="shared" si="3"/>
+        <v>'': 'NONE: Duplicate Row',</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A84" s="2" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I84" xr:uid="{E25534D8-8326-A74F-A2E5-C7F409A5D2ED}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A31:I83">
-      <sortCondition ref="A1:A84"/>
+  <autoFilter ref="A1:J81" xr:uid="{E25534D8-8326-A74F-A2E5-C7F409A5D2ED}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A31:J80">
+      <sortCondition ref="A1:A81"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="D21" r:id="rId1" display="example@gmial.com" xr:uid="{26614BCF-17CC-CC4B-8956-8F6930E60309}"/>
-    <hyperlink ref="E21" r:id="rId2" display="example@gmail.com" xr:uid="{8748665C-4957-DF46-BCAE-78DDC2747FA2}"/>
-    <hyperlink ref="E16" r:id="rId3" xr:uid="{C97D70EF-2237-5345-A311-3AAA5FB2604F}"/>
-    <hyperlink ref="D17" r:id="rId4" xr:uid="{5452BAFC-13C2-3F47-9997-9E87936810D4}"/>
-    <hyperlink ref="E17" r:id="rId5" xr:uid="{26E7AAAB-28B9-3346-B8F0-69E39759EBA8}"/>
-    <hyperlink ref="E19" r:id="rId6" xr:uid="{1E86A40A-BC53-844D-A055-9CA50642AB3B}"/>
+    <hyperlink ref="E21" r:id="rId1" display="example@gmial.com" xr:uid="{26614BCF-17CC-CC4B-8956-8F6930E60309}"/>
+    <hyperlink ref="F21" r:id="rId2" display="example@gmail.com" xr:uid="{8748665C-4957-DF46-BCAE-78DDC2747FA2}"/>
+    <hyperlink ref="F16" r:id="rId3" xr:uid="{C97D70EF-2237-5345-A311-3AAA5FB2604F}"/>
+    <hyperlink ref="E17" r:id="rId4" xr:uid="{5452BAFC-13C2-3F47-9997-9E87936810D4}"/>
+    <hyperlink ref="F17" r:id="rId5" xr:uid="{26E7AAAB-28B9-3346-B8F0-69E39759EBA8}"/>
+    <hyperlink ref="F19" r:id="rId6" xr:uid="{1E86A40A-BC53-844D-A055-9CA50642AB3B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -3123,12 +3679,12 @@
   <sheetData>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
@@ -3138,322 +3694,322 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -3487,7 +4043,7 @@
         <v>1101</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -3495,7 +4051,7 @@
         <v>1102</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -3503,7 +4059,7 @@
         <v>1103</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -3519,7 +4075,7 @@
         <v>1105</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -3527,7 +4083,7 @@
         <v>1106</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -3535,7 +4091,7 @@
         <v>1201</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -3543,7 +4099,7 @@
         <v>1202</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -3559,7 +4115,7 @@
         <v>1204</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -3567,7 +4123,7 @@
         <v>2101</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -3583,7 +4139,7 @@
         <v>2103</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -3591,7 +4147,7 @@
         <v>2104</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -3607,7 +4163,7 @@
         <v>2106</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -3615,7 +4171,7 @@
         <v>2107</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -3623,7 +4179,7 @@
         <v>2108</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -3631,7 +4187,7 @@
         <v>3101</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -3639,7 +4195,7 @@
         <v>3102</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -3647,7 +4203,7 @@
         <v>3103</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -3655,7 +4211,7 @@
         <v>3104</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -3679,7 +4235,7 @@
         <v>3107</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -3687,7 +4243,7 @@
         <v>3108</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -3703,7 +4259,7 @@
         <v>4102</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -3711,7 +4267,7 @@
         <v>4103</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -3719,7 +4275,7 @@
         <v>4104</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -3727,7 +4283,7 @@
         <v>4104</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -3735,7 +4291,7 @@
         <v>4104</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -3743,7 +4299,7 @@
         <v>4105</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -3751,7 +4307,7 @@
         <v>4106</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -3775,7 +4331,7 @@
         <v>4109</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -3791,7 +4347,7 @@
         <v>4111</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -3799,7 +4355,7 @@
         <v>4112</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -3807,7 +4363,7 @@
         <v>4113</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -3815,7 +4371,7 @@
         <v>4113</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
@@ -3831,7 +4387,7 @@
         <v>4113</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
@@ -3847,7 +4403,7 @@
         <v>4202</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -3855,7 +4411,7 @@
         <v>4203</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -3863,7 +4419,7 @@
         <v>4203</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -3871,7 +4427,7 @@
         <v>4203</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -3879,7 +4435,7 @@
         <v>4204</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
@@ -3887,7 +4443,7 @@
         <v>4204</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
@@ -3927,7 +4483,7 @@
         <v>4301</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
@@ -3943,7 +4499,7 @@
         <v>4303</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
@@ -3959,7 +4515,7 @@
         <v>4305</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
@@ -3983,7 +4539,7 @@
         <v>4308</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
@@ -3999,7 +4555,7 @@
         <v>4402</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>